<commit_message>
add result sheet for 30-106
</commit_message>
<xml_diff>
--- a/preliminary-study/first_stratum_raw_result.xlsx
+++ b/preliminary-study/first_stratum_raw_result.xlsx
@@ -603,7 +603,7 @@
         <v>1</v>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2" t="inlineStr">
         <is>
@@ -745,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="T4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4" t="inlineStr">
         <is>
@@ -816,7 +816,7 @@
         <v>1</v>
       </c>
       <c r="T5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5" t="inlineStr">
         <is>
@@ -1526,7 +1526,7 @@
         <v>1</v>
       </c>
       <c r="T15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15" t="inlineStr">
         <is>
@@ -1597,7 +1597,7 @@
         <v>1</v>
       </c>
       <c r="T16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16" t="inlineStr">
         <is>
@@ -1739,7 +1739,7 @@
         <v>1</v>
       </c>
       <c r="T18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18" t="inlineStr">
         <is>
@@ -1881,7 +1881,7 @@
         <v>1</v>
       </c>
       <c r="T20" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U20" t="inlineStr">
         <is>
@@ -1952,7 +1952,7 @@
         <v>1</v>
       </c>
       <c r="T21" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U21" t="inlineStr">
         <is>
@@ -2023,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="T22" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
@@ -2094,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="T23" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
@@ -2165,7 +2165,7 @@
         <v>1</v>
       </c>
       <c r="T24" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U24" t="inlineStr">
         <is>
@@ -2236,7 +2236,7 @@
         <v>1</v>
       </c>
       <c r="T25" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U25" t="inlineStr">
         <is>
@@ -2307,7 +2307,7 @@
         <v>1</v>
       </c>
       <c r="T26" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U26" t="inlineStr">
         <is>
@@ -2378,7 +2378,7 @@
         <v>1</v>
       </c>
       <c r="T27" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U27" t="inlineStr">
         <is>
@@ -2449,7 +2449,7 @@
         <v>1</v>
       </c>
       <c r="T28" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U28" t="inlineStr">
         <is>
@@ -2520,7 +2520,7 @@
         <v>1</v>
       </c>
       <c r="T29" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U29" t="inlineStr">
         <is>
@@ -2591,7 +2591,7 @@
         <v>1</v>
       </c>
       <c r="T30" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U30" t="inlineStr">
         <is>
@@ -2662,7 +2662,7 @@
         <v>1</v>
       </c>
       <c r="T31" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U31" t="inlineStr">
         <is>
@@ -2733,7 +2733,7 @@
         <v>1</v>
       </c>
       <c r="T32" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U32" t="inlineStr">
         <is>
@@ -2804,7 +2804,7 @@
         <v>1</v>
       </c>
       <c r="T33" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U33" t="inlineStr">
         <is>
@@ -2875,7 +2875,7 @@
         <v>1</v>
       </c>
       <c r="T34" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U34" t="inlineStr">
         <is>
@@ -2946,7 +2946,7 @@
         <v>1</v>
       </c>
       <c r="T35" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U35" t="inlineStr">
         <is>
@@ -3017,7 +3017,7 @@
         <v>1</v>
       </c>
       <c r="T36" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U36" t="inlineStr">
         <is>
@@ -3088,7 +3088,7 @@
         <v>1</v>
       </c>
       <c r="T37" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U37" t="inlineStr">
         <is>
@@ -3159,7 +3159,7 @@
         <v>1</v>
       </c>
       <c r="T38" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U38" t="inlineStr">
         <is>
@@ -3230,7 +3230,7 @@
         <v>1</v>
       </c>
       <c r="T39" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U39" t="inlineStr">
         <is>
@@ -3301,7 +3301,7 @@
         <v>1</v>
       </c>
       <c r="T40" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U40" t="inlineStr">
         <is>
@@ -3372,7 +3372,7 @@
         <v>1</v>
       </c>
       <c r="T41" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U41" t="inlineStr">
         <is>
@@ -3443,7 +3443,7 @@
         <v>1</v>
       </c>
       <c r="T42" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U42" t="inlineStr">
         <is>
@@ -3514,7 +3514,7 @@
         <v>1</v>
       </c>
       <c r="T43" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U43" t="inlineStr">
         <is>
@@ -3585,7 +3585,7 @@
         <v>1</v>
       </c>
       <c r="T44" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U44" t="inlineStr">
         <is>
@@ -3656,7 +3656,7 @@
         <v>1</v>
       </c>
       <c r="T45" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U45" t="inlineStr">
         <is>
@@ -3727,7 +3727,7 @@
         <v>1</v>
       </c>
       <c r="T46" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U46" t="inlineStr">
         <is>
@@ -3798,7 +3798,7 @@
         <v>1</v>
       </c>
       <c r="T47" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U47" t="inlineStr">
         <is>
@@ -3869,7 +3869,7 @@
         <v>1</v>
       </c>
       <c r="T48" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U48" t="inlineStr">
         <is>
@@ -3940,7 +3940,7 @@
         <v>1</v>
       </c>
       <c r="T49" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U49" t="inlineStr">
         <is>
@@ -4011,7 +4011,7 @@
         <v>1</v>
       </c>
       <c r="T50" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U50" t="inlineStr">
         <is>
@@ -4082,7 +4082,7 @@
         <v>1</v>
       </c>
       <c r="T51" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U51" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
         <v>1</v>
       </c>
       <c r="T52" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U52" t="inlineStr">
         <is>
@@ -4224,7 +4224,7 @@
         <v>1</v>
       </c>
       <c r="T53" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U53" t="inlineStr">
         <is>
@@ -4295,7 +4295,7 @@
         <v>1</v>
       </c>
       <c r="T54" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U54" t="inlineStr">
         <is>
@@ -4366,7 +4366,7 @@
         <v>1</v>
       </c>
       <c r="T55" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U55" t="inlineStr">
         <is>
@@ -4437,7 +4437,7 @@
         <v>1</v>
       </c>
       <c r="T56" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U56" t="inlineStr">
         <is>
@@ -4508,7 +4508,7 @@
         <v>1</v>
       </c>
       <c r="T57" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U57" t="inlineStr">
         <is>
@@ -4579,7 +4579,7 @@
         <v>1</v>
       </c>
       <c r="T58" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U58" t="inlineStr">
         <is>
@@ -4650,7 +4650,7 @@
         <v>1</v>
       </c>
       <c r="T59" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U59" t="inlineStr">
         <is>
@@ -4721,7 +4721,7 @@
         <v>1</v>
       </c>
       <c r="T60" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U60" t="inlineStr">
         <is>
@@ -4792,7 +4792,7 @@
         <v>1</v>
       </c>
       <c r="T61" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U61" t="inlineStr">
         <is>
@@ -4863,7 +4863,7 @@
         <v>1</v>
       </c>
       <c r="T62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U62" t="inlineStr">
         <is>
@@ -4934,7 +4934,7 @@
         <v>1</v>
       </c>
       <c r="T63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U63" t="inlineStr">
         <is>
@@ -5005,7 +5005,7 @@
         <v>1</v>
       </c>
       <c r="T64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U64" t="inlineStr">
         <is>
@@ -5218,7 +5218,7 @@
         <v>1</v>
       </c>
       <c r="T67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U67" t="inlineStr">
         <is>
@@ -5289,7 +5289,7 @@
         <v>1</v>
       </c>
       <c r="T68" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U68" t="inlineStr">
         <is>
@@ -5360,7 +5360,7 @@
         <v>1</v>
       </c>
       <c r="T69" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U69" t="inlineStr">
         <is>
@@ -5431,7 +5431,7 @@
         <v>1</v>
       </c>
       <c r="T70" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U70" t="inlineStr">
         <is>
@@ -5502,7 +5502,7 @@
         <v>1</v>
       </c>
       <c r="T71" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U71" t="inlineStr">
         <is>
@@ -5573,7 +5573,7 @@
         <v>1</v>
       </c>
       <c r="T72" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U72" t="inlineStr">
         <is>
@@ -5644,7 +5644,7 @@
         <v>1</v>
       </c>
       <c r="T73" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U73" t="inlineStr">
         <is>
@@ -5857,7 +5857,7 @@
         <v>1</v>
       </c>
       <c r="T76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U76" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
         <v>1</v>
       </c>
       <c r="T77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U77" t="inlineStr">
         <is>
@@ -6567,7 +6567,7 @@
         <v>1</v>
       </c>
       <c r="T86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U86" t="inlineStr">
         <is>
@@ -6780,7 +6780,7 @@
         <v>1</v>
       </c>
       <c r="T89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U89" t="inlineStr">
         <is>
@@ -6851,7 +6851,7 @@
         <v>1</v>
       </c>
       <c r="T90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U90" t="inlineStr">
         <is>
@@ -6922,7 +6922,7 @@
         <v>1</v>
       </c>
       <c r="T91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U91" t="inlineStr">
         <is>
@@ -6993,7 +6993,7 @@
         <v>1</v>
       </c>
       <c r="T92" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U92" t="inlineStr">
         <is>
@@ -7064,7 +7064,7 @@
         <v>1</v>
       </c>
       <c r="T93" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U93" t="inlineStr">
         <is>
@@ -7135,7 +7135,7 @@
         <v>1</v>
       </c>
       <c r="T94" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U94" t="inlineStr">
         <is>
@@ -7206,7 +7206,7 @@
         <v>1</v>
       </c>
       <c r="T95" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U95" t="inlineStr">
         <is>
@@ -7277,7 +7277,7 @@
         <v>1</v>
       </c>
       <c r="T96" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
@@ -7348,7 +7348,7 @@
         <v>1</v>
       </c>
       <c r="T97" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U97" t="inlineStr">
         <is>
@@ -7419,7 +7419,7 @@
         <v>1</v>
       </c>
       <c r="T98" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U98" t="inlineStr">
         <is>
@@ -7490,7 +7490,7 @@
         <v>1</v>
       </c>
       <c r="T99" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U99" t="inlineStr">
         <is>
@@ -7561,7 +7561,7 @@
         <v>1</v>
       </c>
       <c r="T100" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U100" t="inlineStr">
         <is>
@@ -7632,7 +7632,7 @@
         <v>1</v>
       </c>
       <c r="T101" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U101" t="inlineStr">
         <is>
@@ -7703,7 +7703,7 @@
         <v>1</v>
       </c>
       <c r="T102" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
@@ -7774,7 +7774,7 @@
         <v>1</v>
       </c>
       <c r="T103" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
@@ -7845,7 +7845,7 @@
         <v>1</v>
       </c>
       <c r="T104" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U104" t="inlineStr">
         <is>
@@ -7916,7 +7916,7 @@
         <v>1</v>
       </c>
       <c r="T105" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U105" t="inlineStr">
         <is>
@@ -7987,7 +7987,7 @@
         <v>1</v>
       </c>
       <c r="T106" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U106" t="inlineStr">
         <is>
@@ -8058,7 +8058,7 @@
         <v>1</v>
       </c>
       <c r="T107" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U107" t="inlineStr">
         <is>
@@ -8129,7 +8129,7 @@
         <v>1</v>
       </c>
       <c r="T108" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U108" t="inlineStr">
         <is>
@@ -8200,7 +8200,7 @@
         <v>1</v>
       </c>
       <c r="T109" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U109" t="inlineStr">
         <is>
@@ -8271,7 +8271,7 @@
         <v>1</v>
       </c>
       <c r="T110" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U110" t="inlineStr">
         <is>
@@ -8342,7 +8342,7 @@
         <v>1</v>
       </c>
       <c r="T111" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U111" t="inlineStr">
         <is>
@@ -8484,7 +8484,7 @@
         <v>1</v>
       </c>
       <c r="T113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U113" t="inlineStr">
         <is>
@@ -8626,7 +8626,7 @@
         <v>1</v>
       </c>
       <c r="T115" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U115" t="inlineStr">
         <is>
@@ -8697,7 +8697,7 @@
         <v>1</v>
       </c>
       <c r="T116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U116" t="inlineStr">
         <is>
@@ -8910,7 +8910,7 @@
         <v>1</v>
       </c>
       <c r="T119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U119" t="inlineStr">
         <is>
@@ -8981,7 +8981,7 @@
         <v>1</v>
       </c>
       <c r="T120" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U120" t="inlineStr">
         <is>
@@ -9194,7 +9194,7 @@
         <v>1</v>
       </c>
       <c r="T123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U123" t="inlineStr">
         <is>
@@ -9336,7 +9336,7 @@
         <v>1</v>
       </c>
       <c r="T125" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U125" t="inlineStr">
         <is>
@@ -9478,7 +9478,7 @@
         <v>1</v>
       </c>
       <c r="T127" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U127" t="inlineStr">
         <is>
@@ -9691,7 +9691,7 @@
         <v>1</v>
       </c>
       <c r="T130" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U130" t="inlineStr">
         <is>
@@ -9833,7 +9833,7 @@
         <v>1</v>
       </c>
       <c r="T132" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U132" t="inlineStr">
         <is>
@@ -10117,7 +10117,7 @@
         <v>1</v>
       </c>
       <c r="T136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U136" t="inlineStr">
         <is>
@@ -10188,7 +10188,7 @@
         <v>1</v>
       </c>
       <c r="T137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U137" t="inlineStr">
         <is>
@@ -10259,7 +10259,7 @@
         <v>1</v>
       </c>
       <c r="T138" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U138" t="inlineStr">
         <is>
@@ -10330,7 +10330,7 @@
         <v>1</v>
       </c>
       <c r="T139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U139" t="inlineStr">
         <is>
@@ -10614,7 +10614,7 @@
         <v>1</v>
       </c>
       <c r="T143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U143" t="inlineStr">
         <is>
@@ -10827,7 +10827,7 @@
         <v>1</v>
       </c>
       <c r="T146" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U146" t="inlineStr">
         <is>
@@ -10898,7 +10898,7 @@
         <v>1</v>
       </c>
       <c r="T147" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U147" t="inlineStr">
         <is>
@@ -10969,7 +10969,7 @@
         <v>1</v>
       </c>
       <c r="T148" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U148" t="inlineStr">
         <is>
@@ -11040,7 +11040,7 @@
         <v>1</v>
       </c>
       <c r="T149" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U149" t="inlineStr">
         <is>
@@ -11111,7 +11111,7 @@
         <v>1</v>
       </c>
       <c r="T150" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U150" t="inlineStr">
         <is>
@@ -11182,7 +11182,7 @@
         <v>1</v>
       </c>
       <c r="T151" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U151" t="inlineStr">
         <is>
@@ -11253,7 +11253,7 @@
         <v>1</v>
       </c>
       <c r="T152" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U152" t="inlineStr">
         <is>
@@ -11324,7 +11324,7 @@
         <v>1</v>
       </c>
       <c r="T153" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U153" t="inlineStr">
         <is>
@@ -11395,7 +11395,7 @@
         <v>1</v>
       </c>
       <c r="T154" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U154" t="inlineStr">
         <is>
@@ -11466,7 +11466,7 @@
         <v>1</v>
       </c>
       <c r="T155" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U155" t="inlineStr">
         <is>
@@ -11537,7 +11537,7 @@
         <v>1</v>
       </c>
       <c r="T156" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U156" t="inlineStr">
         <is>
@@ -11608,7 +11608,7 @@
         <v>1</v>
       </c>
       <c r="T157" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U157" t="inlineStr">
         <is>
@@ -11679,7 +11679,7 @@
         <v>1</v>
       </c>
       <c r="T158" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U158" t="inlineStr">
         <is>
@@ -11750,7 +11750,7 @@
         <v>1</v>
       </c>
       <c r="T159" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U159" t="inlineStr">
         <is>
@@ -11821,7 +11821,7 @@
         <v>1</v>
       </c>
       <c r="T160" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U160" t="inlineStr">
         <is>
@@ -11892,7 +11892,7 @@
         <v>1</v>
       </c>
       <c r="T161" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U161" t="inlineStr">
         <is>
@@ -11963,7 +11963,7 @@
         <v>1</v>
       </c>
       <c r="T162" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U162" t="inlineStr">
         <is>
@@ -12034,7 +12034,7 @@
         <v>1</v>
       </c>
       <c r="T163" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U163" t="inlineStr">
         <is>
@@ -12105,7 +12105,7 @@
         <v>1</v>
       </c>
       <c r="T164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U164" t="inlineStr">
         <is>
@@ -12389,7 +12389,7 @@
         <v>1</v>
       </c>
       <c r="T168" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U168" t="inlineStr">
         <is>
@@ -12460,7 +12460,7 @@
         <v>1</v>
       </c>
       <c r="T169" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U169" t="inlineStr">
         <is>
@@ -12602,7 +12602,7 @@
         <v>1</v>
       </c>
       <c r="T171" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U171" t="inlineStr">
         <is>
@@ -12815,7 +12815,7 @@
         <v>1</v>
       </c>
       <c r="T174" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U174" t="inlineStr">
         <is>
@@ -12886,7 +12886,7 @@
         <v>1</v>
       </c>
       <c r="T175" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U175" t="inlineStr">
         <is>
@@ -12957,7 +12957,7 @@
         <v>1</v>
       </c>
       <c r="T176" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U176" t="inlineStr">
         <is>
@@ -13028,7 +13028,7 @@
         <v>1</v>
       </c>
       <c r="T177" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U177" t="inlineStr">
         <is>
@@ -13099,7 +13099,7 @@
         <v>1</v>
       </c>
       <c r="T178" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U178" t="inlineStr">
         <is>
@@ -13170,7 +13170,7 @@
         <v>1</v>
       </c>
       <c r="T179" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U179" t="inlineStr">
         <is>
@@ -13241,7 +13241,7 @@
         <v>1</v>
       </c>
       <c r="T180" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U180" t="inlineStr">
         <is>
@@ -13312,7 +13312,7 @@
         <v>1</v>
       </c>
       <c r="T181" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U181" t="inlineStr">
         <is>
@@ -13383,7 +13383,7 @@
         <v>1</v>
       </c>
       <c r="T182" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U182" t="inlineStr">
         <is>
@@ -13454,7 +13454,7 @@
         <v>1</v>
       </c>
       <c r="T183" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U183" t="inlineStr">
         <is>
@@ -13525,7 +13525,7 @@
         <v>1</v>
       </c>
       <c r="T184" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U184" t="inlineStr">
         <is>
@@ -13596,7 +13596,7 @@
         <v>1</v>
       </c>
       <c r="T185" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U185" t="inlineStr">
         <is>
@@ -13667,7 +13667,7 @@
         <v>1</v>
       </c>
       <c r="T186" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U186" t="inlineStr">
         <is>
@@ -13738,7 +13738,7 @@
         <v>1</v>
       </c>
       <c r="T187" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U187" t="inlineStr">
         <is>
@@ -13809,7 +13809,7 @@
         <v>1</v>
       </c>
       <c r="T188" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U188" t="inlineStr">
         <is>
@@ -13880,7 +13880,7 @@
         <v>1</v>
       </c>
       <c r="T189" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U189" t="inlineStr">
         <is>
@@ -13951,7 +13951,7 @@
         <v>1</v>
       </c>
       <c r="T190" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U190" t="inlineStr">
         <is>
@@ -14022,7 +14022,7 @@
         <v>1</v>
       </c>
       <c r="T191" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U191" t="inlineStr">
         <is>
@@ -14164,7 +14164,7 @@
         <v>1</v>
       </c>
       <c r="T193" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U193" t="inlineStr">
         <is>
@@ -14235,7 +14235,7 @@
         <v>1</v>
       </c>
       <c r="T194" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U194" t="inlineStr">
         <is>
@@ -14519,7 +14519,7 @@
         <v>1</v>
       </c>
       <c r="T198" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U198" t="inlineStr">
         <is>
@@ -14874,7 +14874,7 @@
         <v>1</v>
       </c>
       <c r="T203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U203" t="inlineStr">
         <is>
@@ -15016,7 +15016,7 @@
         <v>1</v>
       </c>
       <c r="T205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U205" t="inlineStr">
         <is>
@@ -15158,7 +15158,7 @@
         <v>1</v>
       </c>
       <c r="T207" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U207" t="inlineStr">
         <is>
@@ -15300,7 +15300,7 @@
         <v>1</v>
       </c>
       <c r="T209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U209" t="inlineStr">
         <is>
@@ -15442,7 +15442,7 @@
         <v>1</v>
       </c>
       <c r="T211" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U211" t="inlineStr">
         <is>
@@ -15513,7 +15513,7 @@
         <v>1</v>
       </c>
       <c r="T212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U212" t="inlineStr">
         <is>
@@ -15939,7 +15939,7 @@
         <v>1</v>
       </c>
       <c r="T218" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U218" t="inlineStr">
         <is>
@@ -16010,7 +16010,7 @@
         <v>1</v>
       </c>
       <c r="T219" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U219" t="inlineStr">
         <is>
@@ -16223,7 +16223,7 @@
         <v>1</v>
       </c>
       <c r="T222" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U222" t="inlineStr">
         <is>
@@ -16294,7 +16294,7 @@
         <v>1</v>
       </c>
       <c r="T223" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U223" t="inlineStr">
         <is>
@@ -16365,7 +16365,7 @@
         <v>1</v>
       </c>
       <c r="T224" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U224" t="inlineStr">
         <is>
@@ -16507,7 +16507,7 @@
         <v>1</v>
       </c>
       <c r="T226" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U226" t="inlineStr">
         <is>
@@ -16649,7 +16649,7 @@
         <v>1</v>
       </c>
       <c r="T228" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U228" t="inlineStr">
         <is>
@@ -16720,7 +16720,7 @@
         <v>1</v>
       </c>
       <c r="T229" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U229" t="inlineStr">
         <is>
@@ -16862,7 +16862,7 @@
         <v>1</v>
       </c>
       <c r="T231" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U231" t="inlineStr">
         <is>
@@ -17004,7 +17004,7 @@
         <v>1</v>
       </c>
       <c r="T233" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U233" t="inlineStr">
         <is>
@@ -17217,7 +17217,7 @@
         <v>1</v>
       </c>
       <c r="T236" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U236" t="inlineStr">
         <is>
@@ -17359,7 +17359,7 @@
         <v>1</v>
       </c>
       <c r="T238" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U238" t="inlineStr">
         <is>
@@ -17785,7 +17785,7 @@
         <v>1</v>
       </c>
       <c r="T244" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U244" t="inlineStr">
         <is>
@@ -17927,7 +17927,7 @@
         <v>1</v>
       </c>
       <c r="T246" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U246" t="inlineStr">
         <is>
@@ -17998,7 +17998,7 @@
         <v>1</v>
       </c>
       <c r="T247" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U247" t="inlineStr">
         <is>
@@ -18211,7 +18211,7 @@
         <v>1</v>
       </c>
       <c r="T250" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U250" t="inlineStr">
         <is>
@@ -18282,7 +18282,7 @@
         <v>1</v>
       </c>
       <c r="T251" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U251" t="inlineStr">
         <is>
@@ -18495,7 +18495,7 @@
         <v>1</v>
       </c>
       <c r="T254" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U254" t="inlineStr">
         <is>
@@ -18566,7 +18566,7 @@
         <v>1</v>
       </c>
       <c r="T255" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U255" t="inlineStr">
         <is>
@@ -18637,7 +18637,7 @@
         <v>1</v>
       </c>
       <c r="T256" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U256" t="inlineStr">
         <is>
@@ -18708,7 +18708,7 @@
         <v>1</v>
       </c>
       <c r="T257" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U257" t="inlineStr">
         <is>
@@ -18779,7 +18779,7 @@
         <v>1</v>
       </c>
       <c r="T258" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U258" t="inlineStr">
         <is>
@@ -18850,7 +18850,7 @@
         <v>1</v>
       </c>
       <c r="T259" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U259" t="inlineStr">
         <is>
@@ -18921,7 +18921,7 @@
         <v>1</v>
       </c>
       <c r="T260" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U260" t="inlineStr">
         <is>
@@ -18992,7 +18992,7 @@
         <v>1</v>
       </c>
       <c r="T261" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U261" t="inlineStr">
         <is>
@@ -19063,7 +19063,7 @@
         <v>1</v>
       </c>
       <c r="T262" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U262" t="inlineStr">
         <is>
@@ -19134,7 +19134,7 @@
         <v>1</v>
       </c>
       <c r="T263" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U263" t="inlineStr">
         <is>
@@ -19276,7 +19276,7 @@
         <v>1</v>
       </c>
       <c r="T265" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U265" t="inlineStr">
         <is>
@@ -19347,7 +19347,7 @@
         <v>1</v>
       </c>
       <c r="T266" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U266" t="inlineStr">
         <is>
@@ -19418,7 +19418,7 @@
         <v>1</v>
       </c>
       <c r="T267" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U267" t="inlineStr">
         <is>
@@ -19489,7 +19489,7 @@
         <v>1</v>
       </c>
       <c r="T268" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U268" t="inlineStr">
         <is>
@@ -19560,7 +19560,7 @@
         <v>1</v>
       </c>
       <c r="T269" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U269" t="inlineStr">
         <is>
@@ -19631,7 +19631,7 @@
         <v>1</v>
       </c>
       <c r="T270" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U270" t="inlineStr">
         <is>
@@ -19702,7 +19702,7 @@
         <v>1</v>
       </c>
       <c r="T271" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U271" t="inlineStr">
         <is>
@@ -19915,7 +19915,7 @@
         <v>1</v>
       </c>
       <c r="T274" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U274" t="inlineStr">
         <is>
@@ -20199,7 +20199,7 @@
         <v>1</v>
       </c>
       <c r="T278" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U278" t="inlineStr">
         <is>
@@ -20270,7 +20270,7 @@
         <v>1</v>
       </c>
       <c r="T279" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U279" t="inlineStr">
         <is>
@@ -20341,7 +20341,7 @@
         <v>1</v>
       </c>
       <c r="T280" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U280" t="inlineStr">
         <is>
@@ -20483,7 +20483,7 @@
         <v>1</v>
       </c>
       <c r="T282" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U282" t="inlineStr">
         <is>
@@ -20625,7 +20625,7 @@
         <v>1</v>
       </c>
       <c r="T284" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U284" t="inlineStr">
         <is>
@@ -20696,7 +20696,7 @@
         <v>1</v>
       </c>
       <c r="T285" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U285" t="inlineStr">
         <is>
@@ -20767,7 +20767,7 @@
         <v>1</v>
       </c>
       <c r="T286" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U286" t="inlineStr">
         <is>
@@ -20838,7 +20838,7 @@
         <v>1</v>
       </c>
       <c r="T287" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U287" t="inlineStr">
         <is>
@@ -20909,7 +20909,7 @@
         <v>1</v>
       </c>
       <c r="T288" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U288" t="inlineStr">
         <is>
@@ -20980,7 +20980,7 @@
         <v>1</v>
       </c>
       <c r="T289" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U289" t="inlineStr">
         <is>
@@ -21051,7 +21051,7 @@
         <v>1</v>
       </c>
       <c r="T290" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U290" t="inlineStr">
         <is>
@@ -21193,7 +21193,7 @@
         <v>1</v>
       </c>
       <c r="T292" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U292" t="inlineStr">
         <is>
@@ -21335,7 +21335,7 @@
         <v>1</v>
       </c>
       <c r="T294" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U294" t="inlineStr">
         <is>
@@ -21406,7 +21406,7 @@
         <v>1</v>
       </c>
       <c r="T295" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U295" t="inlineStr">
         <is>
@@ -21548,7 +21548,7 @@
         <v>1</v>
       </c>
       <c r="T297" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U297" t="inlineStr">
         <is>
@@ -21690,7 +21690,7 @@
         <v>1</v>
       </c>
       <c r="T299" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U299" t="inlineStr">
         <is>
@@ -21761,7 +21761,7 @@
         <v>1</v>
       </c>
       <c r="T300" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U300" t="inlineStr">
         <is>
@@ -21832,7 +21832,7 @@
         <v>1</v>
       </c>
       <c r="T301" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U301" t="inlineStr">
         <is>
@@ -22045,7 +22045,7 @@
         <v>1</v>
       </c>
       <c r="T304" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U304" t="inlineStr">
         <is>
@@ -22187,7 +22187,7 @@
         <v>1</v>
       </c>
       <c r="T306" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U306" t="inlineStr">
         <is>
@@ -22329,7 +22329,7 @@
         <v>1</v>
       </c>
       <c r="T308" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U308" t="inlineStr">
         <is>
@@ -22400,7 +22400,7 @@
         <v>1</v>
       </c>
       <c r="T309" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U309" t="inlineStr">
         <is>
@@ -22613,7 +22613,7 @@
         <v>1</v>
       </c>
       <c r="T312" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U312" t="inlineStr">
         <is>
@@ -22684,7 +22684,7 @@
         <v>1</v>
       </c>
       <c r="T313" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U313" t="inlineStr">
         <is>
@@ -22755,7 +22755,7 @@
         <v>1</v>
       </c>
       <c r="T314" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U314" t="inlineStr">
         <is>
@@ -22826,7 +22826,7 @@
         <v>1</v>
       </c>
       <c r="T315" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U315" t="inlineStr">
         <is>
@@ -22897,7 +22897,7 @@
         <v>1</v>
       </c>
       <c r="T316" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U316" t="inlineStr">
         <is>
@@ -23039,7 +23039,7 @@
         <v>1</v>
       </c>
       <c r="T318" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U318" t="inlineStr">
         <is>
@@ -23110,7 +23110,7 @@
         <v>1</v>
       </c>
       <c r="T319" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U319" t="inlineStr">
         <is>
@@ -23181,7 +23181,7 @@
         <v>1</v>
       </c>
       <c r="T320" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U320" t="inlineStr">
         <is>
@@ -23252,7 +23252,7 @@
         <v>1</v>
       </c>
       <c r="T321" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U321" t="inlineStr">
         <is>
@@ -23323,7 +23323,7 @@
         <v>1</v>
       </c>
       <c r="T322" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U322" t="inlineStr">
         <is>
@@ -23394,7 +23394,7 @@
         <v>1</v>
       </c>
       <c r="T323" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U323" t="inlineStr">
         <is>
@@ -23465,7 +23465,7 @@
         <v>1</v>
       </c>
       <c r="T324" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U324" t="inlineStr">
         <is>
@@ -23607,7 +23607,7 @@
         <v>1</v>
       </c>
       <c r="T326" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U326" t="inlineStr">
         <is>
@@ -23749,7 +23749,7 @@
         <v>1</v>
       </c>
       <c r="T328" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U328" t="inlineStr">
         <is>
@@ -23962,7 +23962,7 @@
         <v>1</v>
       </c>
       <c r="T331" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U331" t="inlineStr">
         <is>
@@ -24104,7 +24104,7 @@
         <v>1</v>
       </c>
       <c r="T333" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U333" t="inlineStr">
         <is>
@@ -24175,7 +24175,7 @@
         <v>1</v>
       </c>
       <c r="T334" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U334" t="inlineStr">
         <is>
@@ -24246,7 +24246,7 @@
         <v>1</v>
       </c>
       <c r="T335" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U335" t="inlineStr">
         <is>
@@ -24317,7 +24317,7 @@
         <v>1</v>
       </c>
       <c r="T336" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U336" t="inlineStr">
         <is>
@@ -24459,7 +24459,7 @@
         <v>1</v>
       </c>
       <c r="T338" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U338" t="inlineStr">
         <is>
@@ -24530,7 +24530,7 @@
         <v>1</v>
       </c>
       <c r="T339" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U339" t="inlineStr">
         <is>
@@ -24601,7 +24601,7 @@
         <v>1</v>
       </c>
       <c r="T340" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U340" t="inlineStr">
         <is>
@@ -24672,7 +24672,7 @@
         <v>1</v>
       </c>
       <c r="T341" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U341" t="inlineStr">
         <is>
@@ -24885,7 +24885,7 @@
         <v>1</v>
       </c>
       <c r="T344" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U344" t="inlineStr">
         <is>
@@ -24956,7 +24956,7 @@
         <v>1</v>
       </c>
       <c r="T345" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U345" t="inlineStr">
         <is>
@@ -25027,7 +25027,7 @@
         <v>1</v>
       </c>
       <c r="T346" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U346" t="inlineStr">
         <is>
@@ -25098,7 +25098,7 @@
         <v>1</v>
       </c>
       <c r="T347" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U347" t="inlineStr">
         <is>
@@ -25169,7 +25169,7 @@
         <v>1</v>
       </c>
       <c r="T348" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U348" t="inlineStr">
         <is>
@@ -25240,7 +25240,7 @@
         <v>1</v>
       </c>
       <c r="T349" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U349" t="inlineStr">
         <is>
@@ -25311,7 +25311,7 @@
         <v>1</v>
       </c>
       <c r="T350" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U350" t="inlineStr">
         <is>
@@ -25382,7 +25382,7 @@
         <v>1</v>
       </c>
       <c r="T351" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U351" t="inlineStr">
         <is>
@@ -25453,7 +25453,7 @@
         <v>1</v>
       </c>
       <c r="T352" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U352" t="inlineStr">
         <is>
@@ -25524,7 +25524,7 @@
         <v>1</v>
       </c>
       <c r="T353" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U353" t="inlineStr">
         <is>
@@ -25595,7 +25595,7 @@
         <v>1</v>
       </c>
       <c r="T354" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U354" t="inlineStr">
         <is>
@@ -25666,7 +25666,7 @@
         <v>1</v>
       </c>
       <c r="T355" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U355" t="inlineStr">
         <is>
@@ -25737,7 +25737,7 @@
         <v>1</v>
       </c>
       <c r="T356" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U356" t="inlineStr">
         <is>
@@ -25808,7 +25808,7 @@
         <v>1</v>
       </c>
       <c r="T357" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U357" t="inlineStr">
         <is>
@@ -25879,7 +25879,7 @@
         <v>1</v>
       </c>
       <c r="T358" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U358" t="inlineStr">
         <is>
@@ -25950,7 +25950,7 @@
         <v>1</v>
       </c>
       <c r="T359" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U359" t="inlineStr">
         <is>
@@ -26021,7 +26021,7 @@
         <v>1</v>
       </c>
       <c r="T360" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U360" t="inlineStr">
         <is>
@@ -26092,7 +26092,7 @@
         <v>1</v>
       </c>
       <c r="T361" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U361" t="inlineStr">
         <is>
@@ -26163,7 +26163,7 @@
         <v>1</v>
       </c>
       <c r="T362" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U362" t="inlineStr">
         <is>
@@ -26376,7 +26376,7 @@
         <v>1</v>
       </c>
       <c r="T365" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U365" t="inlineStr">
         <is>
@@ -26518,7 +26518,7 @@
         <v>1</v>
       </c>
       <c r="T367" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U367" t="inlineStr">
         <is>
@@ -26731,7 +26731,7 @@
         <v>1</v>
       </c>
       <c r="T370" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U370" t="inlineStr">
         <is>
@@ -27015,7 +27015,7 @@
         <v>1</v>
       </c>
       <c r="T374" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U374" t="inlineStr">
         <is>
@@ -27299,7 +27299,7 @@
         <v>1</v>
       </c>
       <c r="T378" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U378" t="inlineStr">
         <is>
@@ -27370,7 +27370,7 @@
         <v>1</v>
       </c>
       <c r="T379" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U379" t="inlineStr">
         <is>
@@ -27654,7 +27654,7 @@
         <v>1</v>
       </c>
       <c r="T383" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U383" t="inlineStr">
         <is>
@@ -27796,7 +27796,7 @@
         <v>1</v>
       </c>
       <c r="T385" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U385" t="inlineStr">
         <is>
@@ -28151,7 +28151,7 @@
         <v>1</v>
       </c>
       <c r="T390" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U390" t="inlineStr">
         <is>
@@ -28222,7 +28222,7 @@
         <v>1</v>
       </c>
       <c r="T391" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U391" t="inlineStr">
         <is>
@@ -28293,7 +28293,7 @@
         <v>1</v>
       </c>
       <c r="T392" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U392" t="inlineStr">
         <is>
@@ -28435,7 +28435,7 @@
         <v>1</v>
       </c>
       <c r="T394" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U394" t="inlineStr">
         <is>
@@ -28719,7 +28719,7 @@
         <v>1</v>
       </c>
       <c r="T398" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U398" t="inlineStr">
         <is>
@@ -28861,7 +28861,7 @@
         <v>1</v>
       </c>
       <c r="T400" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U400" t="inlineStr">
         <is>
@@ -28932,7 +28932,7 @@
         <v>1</v>
       </c>
       <c r="T401" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U401" t="inlineStr">
         <is>
@@ -29003,7 +29003,7 @@
         <v>1</v>
       </c>
       <c r="T402" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U402" t="inlineStr">
         <is>
@@ -29145,7 +29145,7 @@
         <v>1</v>
       </c>
       <c r="T404" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U404" t="inlineStr">
         <is>
@@ -29500,7 +29500,7 @@
         <v>1</v>
       </c>
       <c r="T409" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U409" t="inlineStr">
         <is>
@@ -29571,7 +29571,7 @@
         <v>1</v>
       </c>
       <c r="T410" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U410" t="inlineStr">
         <is>
@@ -29713,7 +29713,7 @@
         <v>1</v>
       </c>
       <c r="T412" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U412" t="inlineStr">
         <is>
@@ -29784,7 +29784,7 @@
         <v>1</v>
       </c>
       <c r="T413" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U413" t="inlineStr">
         <is>
@@ -29855,7 +29855,7 @@
         <v>1</v>
       </c>
       <c r="T414" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U414" t="inlineStr">
         <is>
@@ -29926,7 +29926,7 @@
         <v>1</v>
       </c>
       <c r="T415" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U415" t="inlineStr">
         <is>
@@ -29997,7 +29997,7 @@
         <v>1</v>
       </c>
       <c r="T416" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U416" t="inlineStr">
         <is>
@@ -30068,7 +30068,7 @@
         <v>1</v>
       </c>
       <c r="T417" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U417" t="inlineStr">
         <is>
@@ -30139,7 +30139,7 @@
         <v>1</v>
       </c>
       <c r="T418" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U418" t="inlineStr">
         <is>
@@ -30210,7 +30210,7 @@
         <v>1</v>
       </c>
       <c r="T419" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U419" t="inlineStr">
         <is>
@@ -30352,7 +30352,7 @@
         <v>1</v>
       </c>
       <c r="T421" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U421" t="inlineStr">
         <is>
@@ -30423,7 +30423,7 @@
         <v>1</v>
       </c>
       <c r="T422" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U422" t="inlineStr">
         <is>
@@ -30494,7 +30494,7 @@
         <v>1</v>
       </c>
       <c r="T423" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U423" t="inlineStr">
         <is>
@@ -30707,7 +30707,7 @@
         <v>1</v>
       </c>
       <c r="T426" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U426" t="inlineStr">
         <is>
@@ -30920,7 +30920,7 @@
         <v>1</v>
       </c>
       <c r="T429" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U429" t="inlineStr">
         <is>
@@ -31062,7 +31062,7 @@
         <v>1</v>
       </c>
       <c r="T431" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U431" t="inlineStr">
         <is>
@@ -31133,7 +31133,7 @@
         <v>1</v>
       </c>
       <c r="T432" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U432" t="inlineStr">
         <is>
@@ -31204,7 +31204,7 @@
         <v>1</v>
       </c>
       <c r="T433" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U433" t="inlineStr">
         <is>
@@ -31346,7 +31346,7 @@
         <v>1</v>
       </c>
       <c r="T435" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U435" t="inlineStr">
         <is>
@@ -31417,7 +31417,7 @@
         <v>1</v>
       </c>
       <c r="T436" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U436" t="inlineStr">
         <is>
@@ -31630,7 +31630,7 @@
         <v>1</v>
       </c>
       <c r="T439" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U439" t="inlineStr">
         <is>
@@ -31701,7 +31701,7 @@
         <v>1</v>
       </c>
       <c r="T440" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U440" t="inlineStr">
         <is>
@@ -31843,7 +31843,7 @@
         <v>1</v>
       </c>
       <c r="T442" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U442" t="inlineStr">
         <is>
@@ -32056,7 +32056,7 @@
         <v>1</v>
       </c>
       <c r="T445" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U445" t="inlineStr">
         <is>
@@ -32127,7 +32127,7 @@
         <v>1</v>
       </c>
       <c r="T446" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U446" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
push result sheet for 30-106
</commit_message>
<xml_diff>
--- a/preliminary-study/first_stratum_raw_result.xlsx
+++ b/preliminary-study/first_stratum_raw_result.xlsx
@@ -1668,7 +1668,7 @@
         <v>1</v>
       </c>
       <c r="T17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U17" t="inlineStr">
         <is>
@@ -2094,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="T23" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
@@ -2165,7 +2165,7 @@
         <v>1</v>
       </c>
       <c r="T24" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U24" t="inlineStr">
         <is>
@@ -2236,7 +2236,7 @@
         <v>1</v>
       </c>
       <c r="T25" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U25" t="inlineStr">
         <is>
@@ -2307,7 +2307,7 @@
         <v>1</v>
       </c>
       <c r="T26" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U26" t="inlineStr">
         <is>
@@ -2378,7 +2378,7 @@
         <v>1</v>
       </c>
       <c r="T27" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U27" t="inlineStr">
         <is>
@@ -2449,7 +2449,7 @@
         <v>1</v>
       </c>
       <c r="T28" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U28" t="inlineStr">
         <is>
@@ -2520,7 +2520,7 @@
         <v>1</v>
       </c>
       <c r="T29" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U29" t="inlineStr">
         <is>
@@ -2591,7 +2591,7 @@
         <v>1</v>
       </c>
       <c r="T30" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U30" t="inlineStr">
         <is>
@@ -2662,7 +2662,7 @@
         <v>1</v>
       </c>
       <c r="T31" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U31" t="inlineStr">
         <is>
@@ -3159,7 +3159,7 @@
         <v>1</v>
       </c>
       <c r="T38" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="U38" t="inlineStr">
         <is>
@@ -3230,7 +3230,7 @@
         <v>1</v>
       </c>
       <c r="T39" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="U39" t="inlineStr">
         <is>
@@ -3301,7 +3301,7 @@
         <v>1</v>
       </c>
       <c r="T40" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U40" t="inlineStr">
         <is>
@@ -3372,7 +3372,7 @@
         <v>1</v>
       </c>
       <c r="T41" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="U41" t="inlineStr">
         <is>
@@ -3443,7 +3443,7 @@
         <v>1</v>
       </c>
       <c r="T42" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="U42" t="inlineStr">
         <is>
@@ -3514,7 +3514,7 @@
         <v>1</v>
       </c>
       <c r="T43" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U43" t="inlineStr">
         <is>
@@ -3585,7 +3585,7 @@
         <v>1</v>
       </c>
       <c r="T44" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U44" t="inlineStr">
         <is>
@@ -3656,7 +3656,7 @@
         <v>1</v>
       </c>
       <c r="T45" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U45" t="inlineStr">
         <is>
@@ -3727,7 +3727,7 @@
         <v>1</v>
       </c>
       <c r="T46" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U46" t="inlineStr">
         <is>
@@ -3798,7 +3798,7 @@
         <v>1</v>
       </c>
       <c r="T47" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U47" t="inlineStr">
         <is>
@@ -3869,7 +3869,7 @@
         <v>1</v>
       </c>
       <c r="T48" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U48" t="inlineStr">
         <is>
@@ -3940,7 +3940,7 @@
         <v>1</v>
       </c>
       <c r="T49" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U49" t="inlineStr">
         <is>
@@ -4011,7 +4011,7 @@
         <v>1</v>
       </c>
       <c r="T50" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="U50" t="inlineStr">
         <is>
@@ -4082,7 +4082,7 @@
         <v>1</v>
       </c>
       <c r="T51" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U51" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
         <v>1</v>
       </c>
       <c r="T52" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U52" t="inlineStr">
         <is>
@@ -4224,7 +4224,7 @@
         <v>1</v>
       </c>
       <c r="T53" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U53" t="inlineStr">
         <is>
@@ -4295,7 +4295,7 @@
         <v>1</v>
       </c>
       <c r="T54" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U54" t="inlineStr">
         <is>
@@ -4366,7 +4366,7 @@
         <v>1</v>
       </c>
       <c r="T55" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U55" t="inlineStr">
         <is>
@@ -4863,7 +4863,7 @@
         <v>1</v>
       </c>
       <c r="T62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U62" t="inlineStr">
         <is>
@@ -4934,7 +4934,7 @@
         <v>1</v>
       </c>
       <c r="T63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U63" t="inlineStr">
         <is>
@@ -5076,7 +5076,7 @@
         <v>1</v>
       </c>
       <c r="T65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U65" t="inlineStr">
         <is>
@@ -5147,7 +5147,7 @@
         <v>1</v>
       </c>
       <c r="T66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U66" t="inlineStr">
         <is>
@@ -5218,7 +5218,7 @@
         <v>1</v>
       </c>
       <c r="T67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U67" t="inlineStr">
         <is>
@@ -5786,7 +5786,7 @@
         <v>1</v>
       </c>
       <c r="T75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U75" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
         <v>1</v>
       </c>
       <c r="T77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U77" t="inlineStr">
         <is>
@@ -6780,7 +6780,7 @@
         <v>1</v>
       </c>
       <c r="T89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U89" t="inlineStr">
         <is>
@@ -6993,7 +6993,7 @@
         <v>1</v>
       </c>
       <c r="T92" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="U92" t="inlineStr">
         <is>
@@ -7064,7 +7064,7 @@
         <v>1</v>
       </c>
       <c r="T93" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U93" t="inlineStr">
         <is>
@@ -7135,7 +7135,7 @@
         <v>1</v>
       </c>
       <c r="T94" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U94" t="inlineStr">
         <is>
@@ -7206,7 +7206,7 @@
         <v>1</v>
       </c>
       <c r="T95" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U95" t="inlineStr">
         <is>
@@ -7277,7 +7277,7 @@
         <v>1</v>
       </c>
       <c r="T96" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
@@ -7348,7 +7348,7 @@
         <v>1</v>
       </c>
       <c r="T97" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U97" t="inlineStr">
         <is>
@@ -7419,7 +7419,7 @@
         <v>1</v>
       </c>
       <c r="T98" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U98" t="inlineStr">
         <is>
@@ -7490,7 +7490,7 @@
         <v>1</v>
       </c>
       <c r="T99" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U99" t="inlineStr">
         <is>
@@ -7561,7 +7561,7 @@
         <v>1</v>
       </c>
       <c r="T100" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U100" t="inlineStr">
         <is>
@@ -7632,7 +7632,7 @@
         <v>1</v>
       </c>
       <c r="T101" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="U101" t="inlineStr">
         <is>
@@ -7703,7 +7703,7 @@
         <v>1</v>
       </c>
       <c r="T102" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
@@ -7774,7 +7774,7 @@
         <v>1</v>
       </c>
       <c r="T103" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
@@ -7845,7 +7845,7 @@
         <v>1</v>
       </c>
       <c r="T104" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U104" t="inlineStr">
         <is>
@@ -7916,7 +7916,7 @@
         <v>1</v>
       </c>
       <c r="T105" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U105" t="inlineStr">
         <is>
@@ -7987,7 +7987,7 @@
         <v>1</v>
       </c>
       <c r="T106" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="U106" t="inlineStr">
         <is>
@@ -8058,7 +8058,7 @@
         <v>1</v>
       </c>
       <c r="T107" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U107" t="inlineStr">
         <is>
@@ -8129,7 +8129,7 @@
         <v>1</v>
       </c>
       <c r="T108" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U108" t="inlineStr">
         <is>
@@ -8200,7 +8200,7 @@
         <v>1</v>
       </c>
       <c r="T109" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U109" t="inlineStr">
         <is>
@@ -8697,7 +8697,7 @@
         <v>1</v>
       </c>
       <c r="T116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U116" t="inlineStr">
         <is>
@@ -8768,7 +8768,7 @@
         <v>1</v>
       </c>
       <c r="T117" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U117" t="inlineStr">
         <is>
@@ -8981,7 +8981,7 @@
         <v>1</v>
       </c>
       <c r="T120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U120" t="inlineStr">
         <is>
@@ -9123,7 +9123,7 @@
         <v>1</v>
       </c>
       <c r="T122" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U122" t="inlineStr">
         <is>
@@ -9407,7 +9407,7 @@
         <v>1</v>
       </c>
       <c r="T126" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U126" t="inlineStr">
         <is>
@@ -9478,7 +9478,7 @@
         <v>1</v>
       </c>
       <c r="T127" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="U127" t="inlineStr">
         <is>
@@ -9691,7 +9691,7 @@
         <v>1</v>
       </c>
       <c r="T130" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U130" t="inlineStr">
         <is>
@@ -9833,7 +9833,7 @@
         <v>1</v>
       </c>
       <c r="T132" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="U132" t="inlineStr">
         <is>
@@ -10117,7 +10117,7 @@
         <v>1</v>
       </c>
       <c r="T136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U136" t="inlineStr">
         <is>
@@ -10259,7 +10259,7 @@
         <v>1</v>
       </c>
       <c r="T138" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U138" t="inlineStr">
         <is>
@@ -10401,7 +10401,7 @@
         <v>1</v>
       </c>
       <c r="T140" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U140" t="inlineStr">
         <is>
@@ -10543,7 +10543,7 @@
         <v>1</v>
       </c>
       <c r="T142" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U142" t="inlineStr">
         <is>
@@ -10614,7 +10614,7 @@
         <v>1</v>
       </c>
       <c r="T143" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U143" t="inlineStr">
         <is>
@@ -10827,7 +10827,7 @@
         <v>1</v>
       </c>
       <c r="T146" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U146" t="inlineStr">
         <is>
@@ -10898,7 +10898,7 @@
         <v>1</v>
       </c>
       <c r="T147" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U147" t="inlineStr">
         <is>
@@ -10969,7 +10969,7 @@
         <v>1</v>
       </c>
       <c r="T148" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U148" t="inlineStr">
         <is>
@@ -11040,7 +11040,7 @@
         <v>1</v>
       </c>
       <c r="T149" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U149" t="inlineStr">
         <is>
@@ -11111,7 +11111,7 @@
         <v>1</v>
       </c>
       <c r="T150" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U150" t="inlineStr">
         <is>
@@ -11182,7 +11182,7 @@
         <v>1</v>
       </c>
       <c r="T151" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U151" t="inlineStr">
         <is>
@@ -11253,7 +11253,7 @@
         <v>1</v>
       </c>
       <c r="T152" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U152" t="inlineStr">
         <is>
@@ -11324,7 +11324,7 @@
         <v>1</v>
       </c>
       <c r="T153" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U153" t="inlineStr">
         <is>
@@ -11395,7 +11395,7 @@
         <v>1</v>
       </c>
       <c r="T154" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U154" t="inlineStr">
         <is>
@@ -11466,7 +11466,7 @@
         <v>1</v>
       </c>
       <c r="T155" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U155" t="inlineStr">
         <is>
@@ -11537,7 +11537,7 @@
         <v>1</v>
       </c>
       <c r="T156" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U156" t="inlineStr">
         <is>
@@ -11608,7 +11608,7 @@
         <v>1</v>
       </c>
       <c r="T157" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U157" t="inlineStr">
         <is>
@@ -11679,7 +11679,7 @@
         <v>1</v>
       </c>
       <c r="T158" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U158" t="inlineStr">
         <is>
@@ -11750,7 +11750,7 @@
         <v>1</v>
       </c>
       <c r="T159" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U159" t="inlineStr">
         <is>
@@ -11821,7 +11821,7 @@
         <v>1</v>
       </c>
       <c r="T160" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U160" t="inlineStr">
         <is>
@@ -11892,7 +11892,7 @@
         <v>1</v>
       </c>
       <c r="T161" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U161" t="inlineStr">
         <is>
@@ -11963,7 +11963,7 @@
         <v>1</v>
       </c>
       <c r="T162" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U162" t="inlineStr">
         <is>
@@ -12034,7 +12034,7 @@
         <v>1</v>
       </c>
       <c r="T163" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U163" t="inlineStr">
         <is>
@@ -12105,7 +12105,7 @@
         <v>1</v>
       </c>
       <c r="T164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U164" t="inlineStr">
         <is>
@@ -12176,7 +12176,7 @@
         <v>1</v>
       </c>
       <c r="T165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U165" t="inlineStr">
         <is>
@@ -12247,7 +12247,7 @@
         <v>1</v>
       </c>
       <c r="T166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U166" t="inlineStr">
         <is>
@@ -12318,7 +12318,7 @@
         <v>1</v>
       </c>
       <c r="T167" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U167" t="inlineStr">
         <is>
@@ -12389,7 +12389,7 @@
         <v>1</v>
       </c>
       <c r="T168" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U168" t="inlineStr">
         <is>
@@ -12460,7 +12460,7 @@
         <v>1</v>
       </c>
       <c r="T169" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U169" t="inlineStr">
         <is>
@@ -12531,7 +12531,7 @@
         <v>1</v>
       </c>
       <c r="T170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U170" t="inlineStr">
         <is>
@@ -12602,7 +12602,7 @@
         <v>1</v>
       </c>
       <c r="T171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U171" t="inlineStr">
         <is>
@@ -12673,7 +12673,7 @@
         <v>1</v>
       </c>
       <c r="T172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U172" t="inlineStr">
         <is>
@@ -12744,7 +12744,7 @@
         <v>1</v>
       </c>
       <c r="T173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U173" t="inlineStr">
         <is>
@@ -12815,7 +12815,7 @@
         <v>1</v>
       </c>
       <c r="T174" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U174" t="inlineStr">
         <is>
@@ -12957,7 +12957,7 @@
         <v>1</v>
       </c>
       <c r="T176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U176" t="inlineStr">
         <is>
@@ -13028,7 +13028,7 @@
         <v>1</v>
       </c>
       <c r="T177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U177" t="inlineStr">
         <is>
@@ -13099,7 +13099,7 @@
         <v>1</v>
       </c>
       <c r="T178" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U178" t="inlineStr">
         <is>
@@ -13383,7 +13383,7 @@
         <v>1</v>
       </c>
       <c r="T182" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U182" t="inlineStr">
         <is>
@@ -13454,7 +13454,7 @@
         <v>1</v>
       </c>
       <c r="T183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U183" t="inlineStr">
         <is>
@@ -13525,7 +13525,7 @@
         <v>1</v>
       </c>
       <c r="T184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U184" t="inlineStr">
         <is>
@@ -13596,7 +13596,7 @@
         <v>1</v>
       </c>
       <c r="T185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U185" t="inlineStr">
         <is>
@@ -13667,7 +13667,7 @@
         <v>1</v>
       </c>
       <c r="T186" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U186" t="inlineStr">
         <is>
@@ -13738,7 +13738,7 @@
         <v>1</v>
       </c>
       <c r="T187" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U187" t="inlineStr">
         <is>
@@ -13809,7 +13809,7 @@
         <v>1</v>
       </c>
       <c r="T188" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U188" t="inlineStr">
         <is>
@@ -13880,7 +13880,7 @@
         <v>1</v>
       </c>
       <c r="T189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U189" t="inlineStr">
         <is>
@@ -13951,7 +13951,7 @@
         <v>1</v>
       </c>
       <c r="T190" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U190" t="inlineStr">
         <is>
@@ -14022,7 +14022,7 @@
         <v>1</v>
       </c>
       <c r="T191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U191" t="inlineStr">
         <is>
@@ -14093,7 +14093,7 @@
         <v>1</v>
       </c>
       <c r="T192" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U192" t="inlineStr">
         <is>
@@ -14235,7 +14235,7 @@
         <v>1</v>
       </c>
       <c r="T194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U194" t="inlineStr">
         <is>
@@ -14306,7 +14306,7 @@
         <v>1</v>
       </c>
       <c r="T195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U195" t="inlineStr">
         <is>
@@ -14377,7 +14377,7 @@
         <v>1</v>
       </c>
       <c r="T196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U196" t="inlineStr">
         <is>
@@ -14448,7 +14448,7 @@
         <v>1</v>
       </c>
       <c r="T197" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U197" t="inlineStr">
         <is>
@@ -14519,7 +14519,7 @@
         <v>1</v>
       </c>
       <c r="T198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U198" t="inlineStr">
         <is>
@@ -14590,7 +14590,7 @@
         <v>1</v>
       </c>
       <c r="T199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U199" t="inlineStr">
         <is>
@@ -14661,7 +14661,7 @@
         <v>1</v>
       </c>
       <c r="T200" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U200" t="inlineStr">
         <is>
@@ -14732,7 +14732,7 @@
         <v>1</v>
       </c>
       <c r="T201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U201" t="inlineStr">
         <is>
@@ -15513,7 +15513,7 @@
         <v>1</v>
       </c>
       <c r="T212" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U212" t="inlineStr">
         <is>
@@ -15797,7 +15797,7 @@
         <v>1</v>
       </c>
       <c r="T216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U216" t="inlineStr">
         <is>
@@ -15868,7 +15868,7 @@
         <v>1</v>
       </c>
       <c r="T217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U217" t="inlineStr">
         <is>
@@ -15939,7 +15939,7 @@
         <v>1</v>
       </c>
       <c r="T218" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U218" t="inlineStr">
         <is>
@@ -16010,7 +16010,7 @@
         <v>1</v>
       </c>
       <c r="T219" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U219" t="inlineStr">
         <is>
@@ -16081,7 +16081,7 @@
         <v>1</v>
       </c>
       <c r="T220" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U220" t="inlineStr">
         <is>
@@ -16152,7 +16152,7 @@
         <v>1</v>
       </c>
       <c r="T221" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U221" t="inlineStr">
         <is>
@@ -16223,7 +16223,7 @@
         <v>1</v>
       </c>
       <c r="T222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U222" t="inlineStr">
         <is>
@@ -16294,7 +16294,7 @@
         <v>1</v>
       </c>
       <c r="T223" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U223" t="inlineStr">
         <is>
@@ -16365,7 +16365,7 @@
         <v>1</v>
       </c>
       <c r="T224" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U224" t="inlineStr">
         <is>
@@ -16436,7 +16436,7 @@
         <v>1</v>
       </c>
       <c r="T225" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U225" t="inlineStr">
         <is>
@@ -16507,7 +16507,7 @@
         <v>1</v>
       </c>
       <c r="T226" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U226" t="inlineStr">
         <is>
@@ -16578,7 +16578,7 @@
         <v>1</v>
       </c>
       <c r="T227" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U227" t="inlineStr">
         <is>
@@ -16649,7 +16649,7 @@
         <v>1</v>
       </c>
       <c r="T228" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U228" t="inlineStr">
         <is>
@@ -16720,7 +16720,7 @@
         <v>1</v>
       </c>
       <c r="T229" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U229" t="inlineStr">
         <is>
@@ -16791,7 +16791,7 @@
         <v>1</v>
       </c>
       <c r="T230" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U230" t="inlineStr">
         <is>
@@ -16862,7 +16862,7 @@
         <v>1</v>
       </c>
       <c r="T231" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U231" t="inlineStr">
         <is>
@@ -16933,7 +16933,7 @@
         <v>1</v>
       </c>
       <c r="T232" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U232" t="inlineStr">
         <is>
@@ -17004,7 +17004,7 @@
         <v>1</v>
       </c>
       <c r="T233" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U233" t="inlineStr">
         <is>
@@ -17075,7 +17075,7 @@
         <v>1</v>
       </c>
       <c r="T234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U234" t="inlineStr">
         <is>
@@ -17146,7 +17146,7 @@
         <v>1</v>
       </c>
       <c r="T235" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U235" t="inlineStr">
         <is>
@@ -17217,7 +17217,7 @@
         <v>1</v>
       </c>
       <c r="T236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U236" t="inlineStr">
         <is>
@@ -17288,7 +17288,7 @@
         <v>1</v>
       </c>
       <c r="T237" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U237" t="inlineStr">
         <is>
@@ -17359,7 +17359,7 @@
         <v>1</v>
       </c>
       <c r="T238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U238" t="inlineStr">
         <is>
@@ -17430,7 +17430,7 @@
         <v>1</v>
       </c>
       <c r="T239" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U239" t="inlineStr">
         <is>
@@ -17501,7 +17501,7 @@
         <v>1</v>
       </c>
       <c r="T240" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U240" t="inlineStr">
         <is>
@@ -17572,7 +17572,7 @@
         <v>1</v>
       </c>
       <c r="T241" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U241" t="inlineStr">
         <is>
@@ -17643,7 +17643,7 @@
         <v>1</v>
       </c>
       <c r="T242" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U242" t="inlineStr">
         <is>
@@ -17714,7 +17714,7 @@
         <v>1</v>
       </c>
       <c r="T243" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U243" t="inlineStr">
         <is>
@@ -17785,7 +17785,7 @@
         <v>1</v>
       </c>
       <c r="T244" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U244" t="inlineStr">
         <is>
@@ -17856,7 +17856,7 @@
         <v>1</v>
       </c>
       <c r="T245" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U245" t="inlineStr">
         <is>
@@ -17927,7 +17927,7 @@
         <v>1</v>
       </c>
       <c r="T246" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U246" t="inlineStr">
         <is>
@@ -17998,7 +17998,7 @@
         <v>1</v>
       </c>
       <c r="T247" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U247" t="inlineStr">
         <is>
@@ -18069,7 +18069,7 @@
         <v>1</v>
       </c>
       <c r="T248" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U248" t="inlineStr">
         <is>
@@ -18140,7 +18140,7 @@
         <v>1</v>
       </c>
       <c r="T249" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U249" t="inlineStr">
         <is>
@@ -18211,7 +18211,7 @@
         <v>1</v>
       </c>
       <c r="T250" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U250" t="inlineStr">
         <is>
@@ -18282,7 +18282,7 @@
         <v>1</v>
       </c>
       <c r="T251" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U251" t="inlineStr">
         <is>
@@ -18353,7 +18353,7 @@
         <v>1</v>
       </c>
       <c r="T252" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U252" t="inlineStr">
         <is>
@@ -18424,7 +18424,7 @@
         <v>1</v>
       </c>
       <c r="T253" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U253" t="inlineStr">
         <is>
@@ -18992,7 +18992,7 @@
         <v>1</v>
       </c>
       <c r="T261" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U261" t="inlineStr">
         <is>
@@ -19063,7 +19063,7 @@
         <v>1</v>
       </c>
       <c r="T262" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U262" t="inlineStr">
         <is>
@@ -19134,7 +19134,7 @@
         <v>1</v>
       </c>
       <c r="T263" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U263" t="inlineStr">
         <is>
@@ -19205,7 +19205,7 @@
         <v>1</v>
       </c>
       <c r="T264" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U264" t="inlineStr">
         <is>
@@ -19276,7 +19276,7 @@
         <v>1</v>
       </c>
       <c r="T265" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U265" t="inlineStr">
         <is>
@@ -19773,7 +19773,7 @@
         <v>1</v>
       </c>
       <c r="T272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U272" t="inlineStr">
         <is>
@@ -19844,7 +19844,7 @@
         <v>1</v>
       </c>
       <c r="T273" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U273" t="inlineStr">
         <is>
@@ -19915,7 +19915,7 @@
         <v>1</v>
       </c>
       <c r="T274" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U274" t="inlineStr">
         <is>
@@ -19986,7 +19986,7 @@
         <v>1</v>
       </c>
       <c r="T275" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U275" t="inlineStr">
         <is>
@@ -20057,7 +20057,7 @@
         <v>1</v>
       </c>
       <c r="T276" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U276" t="inlineStr">
         <is>
@@ -20128,7 +20128,7 @@
         <v>1</v>
       </c>
       <c r="T277" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U277" t="inlineStr">
         <is>
@@ -20199,7 +20199,7 @@
         <v>1</v>
       </c>
       <c r="T278" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U278" t="inlineStr">
         <is>
@@ -20270,7 +20270,7 @@
         <v>1</v>
       </c>
       <c r="T279" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U279" t="inlineStr">
         <is>
@@ -20412,7 +20412,7 @@
         <v>1</v>
       </c>
       <c r="T281" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U281" t="inlineStr">
         <is>
@@ -20483,7 +20483,7 @@
         <v>1</v>
       </c>
       <c r="T282" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U282" t="inlineStr">
         <is>
@@ -20554,7 +20554,7 @@
         <v>1</v>
       </c>
       <c r="T283" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U283" t="inlineStr">
         <is>
@@ -20625,7 +20625,7 @@
         <v>1</v>
       </c>
       <c r="T284" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U284" t="inlineStr">
         <is>
@@ -20838,7 +20838,7 @@
         <v>1</v>
       </c>
       <c r="T287" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U287" t="inlineStr">
         <is>
@@ -20909,7 +20909,7 @@
         <v>1</v>
       </c>
       <c r="T288" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U288" t="inlineStr">
         <is>
@@ -20980,7 +20980,7 @@
         <v>1</v>
       </c>
       <c r="T289" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U289" t="inlineStr">
         <is>
@@ -21051,7 +21051,7 @@
         <v>1</v>
       </c>
       <c r="T290" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U290" t="inlineStr">
         <is>
@@ -21122,7 +21122,7 @@
         <v>1</v>
       </c>
       <c r="T291" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U291" t="inlineStr">
         <is>
@@ -21193,7 +21193,7 @@
         <v>1</v>
       </c>
       <c r="T292" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U292" t="inlineStr">
         <is>
@@ -21264,7 +21264,7 @@
         <v>1</v>
       </c>
       <c r="T293" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U293" t="inlineStr">
         <is>
@@ -21335,7 +21335,7 @@
         <v>1</v>
       </c>
       <c r="T294" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U294" t="inlineStr">
         <is>
@@ -21406,7 +21406,7 @@
         <v>1</v>
       </c>
       <c r="T295" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U295" t="inlineStr">
         <is>
@@ -21477,7 +21477,7 @@
         <v>1</v>
       </c>
       <c r="T296" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U296" t="inlineStr">
         <is>
@@ -21619,7 +21619,7 @@
         <v>1</v>
       </c>
       <c r="T298" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U298" t="inlineStr">
         <is>
@@ -21690,7 +21690,7 @@
         <v>1</v>
       </c>
       <c r="T299" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U299" t="inlineStr">
         <is>
@@ -21761,7 +21761,7 @@
         <v>1</v>
       </c>
       <c r="T300" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U300" t="inlineStr">
         <is>
@@ -21832,7 +21832,7 @@
         <v>1</v>
       </c>
       <c r="T301" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U301" t="inlineStr">
         <is>
@@ -21903,7 +21903,7 @@
         <v>1</v>
       </c>
       <c r="T302" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U302" t="inlineStr">
         <is>
@@ -21974,7 +21974,7 @@
         <v>1</v>
       </c>
       <c r="T303" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U303" t="inlineStr">
         <is>
@@ -22045,7 +22045,7 @@
         <v>1</v>
       </c>
       <c r="T304" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U304" t="inlineStr">
         <is>
@@ -22116,7 +22116,7 @@
         <v>1</v>
       </c>
       <c r="T305" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U305" t="inlineStr">
         <is>
@@ -22187,7 +22187,7 @@
         <v>1</v>
       </c>
       <c r="T306" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U306" t="inlineStr">
         <is>
@@ -22258,7 +22258,7 @@
         <v>1</v>
       </c>
       <c r="T307" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U307" t="inlineStr">
         <is>
@@ -22329,7 +22329,7 @@
         <v>1</v>
       </c>
       <c r="T308" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U308" t="inlineStr">
         <is>
@@ -22400,7 +22400,7 @@
         <v>1</v>
       </c>
       <c r="T309" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U309" t="inlineStr">
         <is>
@@ -22471,7 +22471,7 @@
         <v>1</v>
       </c>
       <c r="T310" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U310" t="inlineStr">
         <is>
@@ -22542,7 +22542,7 @@
         <v>1</v>
       </c>
       <c r="T311" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U311" t="inlineStr">
         <is>
@@ -22613,7 +22613,7 @@
         <v>1</v>
       </c>
       <c r="T312" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U312" t="inlineStr">
         <is>
@@ -22684,7 +22684,7 @@
         <v>1</v>
       </c>
       <c r="T313" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U313" t="inlineStr">
         <is>
@@ -22755,7 +22755,7 @@
         <v>1</v>
       </c>
       <c r="T314" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U314" t="inlineStr">
         <is>
@@ -22826,7 +22826,7 @@
         <v>1</v>
       </c>
       <c r="T315" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U315" t="inlineStr">
         <is>
@@ -22897,7 +22897,7 @@
         <v>1</v>
       </c>
       <c r="T316" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U316" t="inlineStr">
         <is>
@@ -22968,7 +22968,7 @@
         <v>1</v>
       </c>
       <c r="T317" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U317" t="inlineStr">
         <is>
@@ -23039,7 +23039,7 @@
         <v>1</v>
       </c>
       <c r="T318" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U318" t="inlineStr">
         <is>
@@ -23110,7 +23110,7 @@
         <v>1</v>
       </c>
       <c r="T319" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U319" t="inlineStr">
         <is>
@@ -23181,7 +23181,7 @@
         <v>1</v>
       </c>
       <c r="T320" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U320" t="inlineStr">
         <is>
@@ -23252,7 +23252,7 @@
         <v>1</v>
       </c>
       <c r="T321" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U321" t="inlineStr">
         <is>
@@ -23323,7 +23323,7 @@
         <v>1</v>
       </c>
       <c r="T322" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U322" t="inlineStr">
         <is>
@@ -23394,7 +23394,7 @@
         <v>1</v>
       </c>
       <c r="T323" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U323" t="inlineStr">
         <is>
@@ -23465,7 +23465,7 @@
         <v>1</v>
       </c>
       <c r="T324" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U324" t="inlineStr">
         <is>
@@ -23536,7 +23536,7 @@
         <v>1</v>
       </c>
       <c r="T325" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U325" t="inlineStr">
         <is>
@@ -23607,7 +23607,7 @@
         <v>1</v>
       </c>
       <c r="T326" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U326" t="inlineStr">
         <is>
@@ -23678,7 +23678,7 @@
         <v>1</v>
       </c>
       <c r="T327" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U327" t="inlineStr">
         <is>
@@ -23749,7 +23749,7 @@
         <v>1</v>
       </c>
       <c r="T328" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U328" t="inlineStr">
         <is>
@@ -23820,7 +23820,7 @@
         <v>1</v>
       </c>
       <c r="T329" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U329" t="inlineStr">
         <is>
@@ -23891,7 +23891,7 @@
         <v>1</v>
       </c>
       <c r="T330" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U330" t="inlineStr">
         <is>
@@ -23962,7 +23962,7 @@
         <v>1</v>
       </c>
       <c r="T331" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U331" t="inlineStr">
         <is>
@@ -24033,7 +24033,7 @@
         <v>1</v>
       </c>
       <c r="T332" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U332" t="inlineStr">
         <is>
@@ -24104,7 +24104,7 @@
         <v>1</v>
       </c>
       <c r="T333" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="U333" t="inlineStr">
         <is>
@@ -24175,7 +24175,7 @@
         <v>1</v>
       </c>
       <c r="T334" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U334" t="inlineStr">
         <is>
@@ -24246,7 +24246,7 @@
         <v>1</v>
       </c>
       <c r="T335" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U335" t="inlineStr">
         <is>
@@ -24317,7 +24317,7 @@
         <v>1</v>
       </c>
       <c r="T336" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U336" t="inlineStr">
         <is>
@@ -24388,7 +24388,7 @@
         <v>1</v>
       </c>
       <c r="T337" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U337" t="inlineStr">
         <is>
@@ -24459,7 +24459,7 @@
         <v>1</v>
       </c>
       <c r="T338" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U338" t="inlineStr">
         <is>
@@ -24530,7 +24530,7 @@
         <v>1</v>
       </c>
       <c r="T339" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U339" t="inlineStr">
         <is>
@@ -24601,7 +24601,7 @@
         <v>1</v>
       </c>
       <c r="T340" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U340" t="inlineStr">
         <is>
@@ -24672,7 +24672,7 @@
         <v>1</v>
       </c>
       <c r="T341" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U341" t="inlineStr">
         <is>
@@ -24743,7 +24743,7 @@
         <v>1</v>
       </c>
       <c r="T342" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U342" t="inlineStr">
         <is>
@@ -24814,7 +24814,7 @@
         <v>1</v>
       </c>
       <c r="T343" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U343" t="inlineStr">
         <is>
@@ -24885,7 +24885,7 @@
         <v>1</v>
       </c>
       <c r="T344" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U344" t="inlineStr">
         <is>
@@ -24956,7 +24956,7 @@
         <v>1</v>
       </c>
       <c r="T345" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U345" t="inlineStr">
         <is>
@@ -25027,7 +25027,7 @@
         <v>1</v>
       </c>
       <c r="T346" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U346" t="inlineStr">
         <is>
@@ -25098,7 +25098,7 @@
         <v>1</v>
       </c>
       <c r="T347" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U347" t="inlineStr">
         <is>
@@ -25169,7 +25169,7 @@
         <v>1</v>
       </c>
       <c r="T348" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U348" t="inlineStr">
         <is>
@@ -25240,7 +25240,7 @@
         <v>1</v>
       </c>
       <c r="T349" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U349" t="inlineStr">
         <is>
@@ -25311,7 +25311,7 @@
         <v>1</v>
       </c>
       <c r="T350" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U350" t="inlineStr">
         <is>
@@ -25382,7 +25382,7 @@
         <v>1</v>
       </c>
       <c r="T351" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U351" t="inlineStr">
         <is>
@@ -25453,7 +25453,7 @@
         <v>1</v>
       </c>
       <c r="T352" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U352" t="inlineStr">
         <is>
@@ -25524,7 +25524,7 @@
         <v>1</v>
       </c>
       <c r="T353" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U353" t="inlineStr">
         <is>
@@ -25595,7 +25595,7 @@
         <v>1</v>
       </c>
       <c r="T354" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U354" t="inlineStr">
         <is>
@@ -25666,7 +25666,7 @@
         <v>1</v>
       </c>
       <c r="T355" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U355" t="inlineStr">
         <is>
@@ -25737,7 +25737,7 @@
         <v>1</v>
       </c>
       <c r="T356" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U356" t="inlineStr">
         <is>
@@ -25808,7 +25808,7 @@
         <v>1</v>
       </c>
       <c r="T357" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U357" t="inlineStr">
         <is>
@@ -25879,7 +25879,7 @@
         <v>1</v>
       </c>
       <c r="T358" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U358" t="inlineStr">
         <is>
@@ -25950,7 +25950,7 @@
         <v>1</v>
       </c>
       <c r="T359" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U359" t="inlineStr">
         <is>
@@ -26021,7 +26021,7 @@
         <v>1</v>
       </c>
       <c r="T360" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U360" t="inlineStr">
         <is>
@@ -26092,7 +26092,7 @@
         <v>1</v>
       </c>
       <c r="T361" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U361" t="inlineStr">
         <is>
@@ -26163,7 +26163,7 @@
         <v>1</v>
       </c>
       <c r="T362" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U362" t="inlineStr">
         <is>
@@ -26589,7 +26589,7 @@
         <v>1</v>
       </c>
       <c r="T368" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U368" t="inlineStr">
         <is>
@@ -26802,7 +26802,7 @@
         <v>1</v>
       </c>
       <c r="T371" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U371" t="inlineStr">
         <is>
@@ -26873,7 +26873,7 @@
         <v>1</v>
       </c>
       <c r="T372" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U372" t="inlineStr">
         <is>
@@ -26944,7 +26944,7 @@
         <v>1</v>
       </c>
       <c r="T373" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U373" t="inlineStr">
         <is>
@@ -27086,7 +27086,7 @@
         <v>1</v>
       </c>
       <c r="T375" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U375" t="inlineStr">
         <is>
@@ -27157,7 +27157,7 @@
         <v>1</v>
       </c>
       <c r="T376" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U376" t="inlineStr">
         <is>
@@ -27441,7 +27441,7 @@
         <v>1</v>
       </c>
       <c r="T380" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U380" t="inlineStr">
         <is>
@@ -27512,7 +27512,7 @@
         <v>1</v>
       </c>
       <c r="T381" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U381" t="inlineStr">
         <is>
@@ -27583,7 +27583,7 @@
         <v>1</v>
       </c>
       <c r="T382" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U382" t="inlineStr">
         <is>
@@ -27796,7 +27796,7 @@
         <v>1</v>
       </c>
       <c r="T385" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U385" t="inlineStr">
         <is>
@@ -27867,7 +27867,7 @@
         <v>1</v>
       </c>
       <c r="T386" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U386" t="inlineStr">
         <is>
@@ -28009,7 +28009,7 @@
         <v>1</v>
       </c>
       <c r="T388" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U388" t="inlineStr">
         <is>
@@ -28151,7 +28151,7 @@
         <v>1</v>
       </c>
       <c r="T390" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U390" t="inlineStr">
         <is>
@@ -28222,7 +28222,7 @@
         <v>1</v>
       </c>
       <c r="T391" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U391" t="inlineStr">
         <is>
@@ -28293,7 +28293,7 @@
         <v>1</v>
       </c>
       <c r="T392" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U392" t="inlineStr">
         <is>
@@ -28435,7 +28435,7 @@
         <v>1</v>
       </c>
       <c r="T394" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U394" t="inlineStr">
         <is>
@@ -28861,7 +28861,7 @@
         <v>1</v>
       </c>
       <c r="T400" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U400" t="inlineStr">
         <is>
@@ -29003,7 +29003,7 @@
         <v>1</v>
       </c>
       <c r="T402" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U402" t="inlineStr">
         <is>
@@ -29287,7 +29287,7 @@
         <v>1</v>
       </c>
       <c r="T406" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U406" t="inlineStr">
         <is>
@@ -29500,7 +29500,7 @@
         <v>1</v>
       </c>
       <c r="T409" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U409" t="inlineStr">
         <is>
@@ -29571,7 +29571,7 @@
         <v>1</v>
       </c>
       <c r="T410" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U410" t="inlineStr">
         <is>
@@ -29997,7 +29997,7 @@
         <v>1</v>
       </c>
       <c r="T416" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U416" t="inlineStr">
         <is>
@@ -30139,7 +30139,7 @@
         <v>1</v>
       </c>
       <c r="T418" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U418" t="inlineStr">
         <is>
@@ -30352,7 +30352,7 @@
         <v>1</v>
       </c>
       <c r="T421" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U421" t="inlineStr">
         <is>
@@ -30636,7 +30636,7 @@
         <v>1</v>
       </c>
       <c r="T425" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U425" t="inlineStr">
         <is>
@@ -30778,7 +30778,7 @@
         <v>1</v>
       </c>
       <c r="T427" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U427" t="inlineStr">
         <is>
@@ -30849,7 +30849,7 @@
         <v>1</v>
       </c>
       <c r="T428" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U428" t="inlineStr">
         <is>
@@ -30991,7 +30991,7 @@
         <v>1</v>
       </c>
       <c r="T430" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U430" t="inlineStr">
         <is>
@@ -31133,7 +31133,7 @@
         <v>1</v>
       </c>
       <c r="T432" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U432" t="inlineStr">
         <is>
@@ -31275,7 +31275,7 @@
         <v>1</v>
       </c>
       <c r="T434" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U434" t="inlineStr">
         <is>
@@ -31346,7 +31346,7 @@
         <v>1</v>
       </c>
       <c r="T435" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U435" t="inlineStr">
         <is>
@@ -31417,7 +31417,7 @@
         <v>1</v>
       </c>
       <c r="T436" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U436" t="inlineStr">
         <is>
@@ -31488,7 +31488,7 @@
         <v>1</v>
       </c>
       <c r="T437" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U437" t="inlineStr">
         <is>
@@ -31559,7 +31559,7 @@
         <v>1</v>
       </c>
       <c r="T438" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U438" t="inlineStr">
         <is>
@@ -31630,7 +31630,7 @@
         <v>1</v>
       </c>
       <c r="T439" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U439" t="inlineStr">
         <is>
@@ -31701,7 +31701,7 @@
         <v>1</v>
       </c>
       <c r="T440" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U440" t="inlineStr">
         <is>
@@ -31772,7 +31772,7 @@
         <v>1</v>
       </c>
       <c r="T441" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U441" t="inlineStr">
         <is>
@@ -31843,7 +31843,7 @@
         <v>1</v>
       </c>
       <c r="T442" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U442" t="inlineStr">
         <is>
@@ -31914,7 +31914,7 @@
         <v>1</v>
       </c>
       <c r="T443" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U443" t="inlineStr">
         <is>
@@ -31985,7 +31985,7 @@
         <v>1</v>
       </c>
       <c r="T444" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U444" t="inlineStr">
         <is>
@@ -32056,7 +32056,7 @@
         <v>1</v>
       </c>
       <c r="T445" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U445" t="inlineStr">
         <is>
@@ -32340,7 +32340,7 @@
         <v>1</v>
       </c>
       <c r="T449" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U449" t="inlineStr">
         <is>
@@ -32411,7 +32411,7 @@
         <v>1</v>
       </c>
       <c r="T450" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U450" t="inlineStr">
         <is>

</xml_diff>